<commit_message>
First serial send prototype
</commit_message>
<xml_diff>
--- a/Mega and MCP pin map.xlsx
+++ b/Mega and MCP pin map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Google Drive\Share\Arduino\G1000_PFD_Mega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA69C7D-CA16-42E9-9FA4-2AD0F25F975F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA55A059-B337-45DB-8477-C640603F46F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,6 +1247,9 @@
       <c r="A36">
         <v>1</v>
       </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
       <c r="C36" t="s">
         <v>9</v>
       </c>
@@ -1261,6 +1264,9 @@
       <c r="A37">
         <v>2</v>
       </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
@@ -1275,6 +1281,9 @@
       <c r="A38">
         <v>3</v>
       </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
       <c r="C38" t="s">
         <v>11</v>
       </c>
@@ -1289,6 +1298,9 @@
       <c r="A39">
         <v>4</v>
       </c>
+      <c r="B39">
+        <v>11</v>
+      </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
@@ -1303,6 +1315,9 @@
       <c r="A40">
         <v>5</v>
       </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
@@ -1317,6 +1332,9 @@
       <c r="A41">
         <v>6</v>
       </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
@@ -1331,6 +1349,9 @@
       <c r="A42">
         <v>7</v>
       </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
       <c r="C42" t="s">
         <v>15</v>
       </c>
@@ -1345,6 +1366,9 @@
       <c r="A43">
         <v>8</v>
       </c>
+      <c r="B43">
+        <v>15</v>
+      </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
@@ -1359,6 +1383,9 @@
       <c r="A44">
         <v>21</v>
       </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
@@ -1373,6 +1400,9 @@
       <c r="A45">
         <v>22</v>
       </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
       <c r="C45" t="s">
         <v>17</v>
       </c>
@@ -1387,6 +1417,9 @@
       <c r="A46">
         <v>23</v>
       </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
@@ -1401,6 +1434,9 @@
       <c r="A47">
         <v>24</v>
       </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
       <c r="C47" t="s">
         <v>20</v>
       </c>
@@ -1415,6 +1451,9 @@
       <c r="A48">
         <v>25</v>
       </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
       <c r="C48" t="s">
         <v>21</v>
       </c>
@@ -1428,6 +1467,9 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>26</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
       </c>
       <c r="C49" t="s">
         <v>22</v>
@@ -1443,6 +1485,9 @@
       <c r="A50">
         <v>27</v>
       </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
       <c r="C50" t="s">
         <v>23</v>
       </c>
@@ -1457,6 +1502,9 @@
       <c r="A51">
         <v>28</v>
       </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
       <c r="C51" t="s">
         <v>24</v>
       </c>
@@ -1496,6 +1544,9 @@
       <c r="A55">
         <v>1</v>
       </c>
+      <c r="B55">
+        <v>8</v>
+      </c>
       <c r="C55" t="s">
         <v>9</v>
       </c>
@@ -1510,6 +1561,9 @@
       <c r="A56">
         <v>2</v>
       </c>
+      <c r="B56">
+        <v>9</v>
+      </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
@@ -1524,6 +1578,9 @@
       <c r="A57">
         <v>3</v>
       </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
       <c r="C57" t="s">
         <v>11</v>
       </c>
@@ -1538,6 +1595,9 @@
       <c r="A58">
         <v>4</v>
       </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
       <c r="C58" t="s">
         <v>12</v>
       </c>
@@ -1552,6 +1612,9 @@
       <c r="A59">
         <v>5</v>
       </c>
+      <c r="B59">
+        <v>12</v>
+      </c>
       <c r="C59" t="s">
         <v>13</v>
       </c>
@@ -1566,6 +1629,9 @@
       <c r="A60">
         <v>6</v>
       </c>
+      <c r="B60">
+        <v>13</v>
+      </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
@@ -1580,6 +1646,9 @@
       <c r="A61">
         <v>7</v>
       </c>
+      <c r="B61">
+        <v>14</v>
+      </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
@@ -1594,6 +1663,9 @@
       <c r="A62">
         <v>8</v>
       </c>
+      <c r="B62">
+        <v>15</v>
+      </c>
       <c r="C62" t="s">
         <v>16</v>
       </c>
@@ -1608,6 +1680,9 @@
       <c r="A63">
         <v>21</v>
       </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
       <c r="C63" t="s">
         <v>18</v>
       </c>
@@ -1622,6 +1697,9 @@
       <c r="A64">
         <v>22</v>
       </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
       <c r="C64" t="s">
         <v>17</v>
       </c>
@@ -1636,6 +1714,9 @@
       <c r="A65">
         <v>23</v>
       </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
       <c r="C65" t="s">
         <v>19</v>
       </c>
@@ -1650,6 +1731,9 @@
       <c r="A66">
         <v>24</v>
       </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
       <c r="C66" t="s">
         <v>20</v>
       </c>
@@ -1664,6 +1748,9 @@
       <c r="A67">
         <v>25</v>
       </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
       <c r="C67" t="s">
         <v>21</v>
       </c>
@@ -1677,6 +1764,9 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>26</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
       </c>
       <c r="C68" t="s">
         <v>22</v>
@@ -1692,6 +1782,9 @@
       <c r="A69">
         <v>27</v>
       </c>
+      <c r="B69">
+        <v>6</v>
+      </c>
       <c r="C69" t="s">
         <v>23</v>
       </c>
@@ -1706,6 +1799,9 @@
       <c r="A70">
         <v>28</v>
       </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
       <c r="C70" t="s">
         <v>24</v>
       </c>
@@ -1745,6 +1841,9 @@
       <c r="A74">
         <v>1</v>
       </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
       <c r="C74" t="s">
         <v>9</v>
       </c>
@@ -1759,6 +1858,9 @@
       <c r="A75">
         <v>2</v>
       </c>
+      <c r="B75">
+        <v>9</v>
+      </c>
       <c r="C75" t="s">
         <v>10</v>
       </c>
@@ -1773,6 +1875,9 @@
       <c r="A76">
         <v>3</v>
       </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
       <c r="C76" t="s">
         <v>11</v>
       </c>
@@ -1787,6 +1892,9 @@
       <c r="A77">
         <v>4</v>
       </c>
+      <c r="B77">
+        <v>11</v>
+      </c>
       <c r="C77" t="s">
         <v>12</v>
       </c>
@@ -1801,6 +1909,9 @@
       <c r="A78">
         <v>5</v>
       </c>
+      <c r="B78">
+        <v>12</v>
+      </c>
       <c r="C78" t="s">
         <v>13</v>
       </c>
@@ -1815,6 +1926,9 @@
       <c r="A79">
         <v>6</v>
       </c>
+      <c r="B79">
+        <v>13</v>
+      </c>
       <c r="C79" t="s">
         <v>14</v>
       </c>
@@ -1829,6 +1943,9 @@
       <c r="A80">
         <v>7</v>
       </c>
+      <c r="B80">
+        <v>14</v>
+      </c>
       <c r="C80" t="s">
         <v>15</v>
       </c>
@@ -1843,6 +1960,9 @@
       <c r="A81">
         <v>8</v>
       </c>
+      <c r="B81">
+        <v>15</v>
+      </c>
       <c r="C81" t="s">
         <v>16</v>
       </c>
@@ -1857,6 +1977,9 @@
       <c r="A82">
         <v>21</v>
       </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
       <c r="C82" t="s">
         <v>18</v>
       </c>
@@ -1871,6 +1994,9 @@
       <c r="A83">
         <v>22</v>
       </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
       <c r="C83" t="s">
         <v>17</v>
       </c>
@@ -1885,6 +2011,9 @@
       <c r="A84">
         <v>23</v>
       </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
       <c r="C84" t="s">
         <v>19</v>
       </c>
@@ -1899,6 +2028,9 @@
       <c r="A85">
         <v>24</v>
       </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
       <c r="C85" t="s">
         <v>20</v>
       </c>
@@ -1913,6 +2045,9 @@
       <c r="A86">
         <v>25</v>
       </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
       <c r="C86" t="s">
         <v>21</v>
       </c>
@@ -1926,6 +2061,9 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>26</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
       </c>
       <c r="C87" t="s">
         <v>22</v>
@@ -1941,6 +2079,9 @@
       <c r="A88">
         <v>27</v>
       </c>
+      <c r="B88">
+        <v>6</v>
+      </c>
       <c r="C88" t="s">
         <v>23</v>
       </c>
@@ -1954,6 +2095,9 @@
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
       </c>
       <c r="C89" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Removed PFD/MFD selection. Added new columns in pin map
</commit_message>
<xml_diff>
--- a/Mega and MCP pin map.xlsx
+++ b/Mega and MCP pin map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Google Drive\Share\Arduino\G1000_PFD_Mega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA55A059-B337-45DB-8477-C640603F46F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01057BE0-88E9-4865-821E-69C48E6AB799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="231">
   <si>
     <t>Arduino pin</t>
   </si>
@@ -433,6 +433,291 @@
   </si>
   <si>
     <t>SOFT_1</t>
+  </si>
+  <si>
+    <t>RSG Command</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_1</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_4</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_3</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_2</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_6</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_5</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_7</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_8</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_9</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_10</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_11</t>
+  </si>
+  <si>
+    <t>BTN_SOFT_12</t>
+  </si>
+  <si>
+    <t>BTN_AP</t>
+  </si>
+  <si>
+    <t>BTN_FD</t>
+  </si>
+  <si>
+    <t>BTN_ALT</t>
+  </si>
+  <si>
+    <t>BTN_HDG</t>
+  </si>
+  <si>
+    <t>BTN_VNAV</t>
+  </si>
+  <si>
+    <t>BTN_NAV</t>
+  </si>
+  <si>
+    <t>BTN_BC</t>
+  </si>
+  <si>
+    <t>BTN_NOSE_UP</t>
+  </si>
+  <si>
+    <t>BTN_APR</t>
+  </si>
+  <si>
+    <t>BTN_VS</t>
+  </si>
+  <si>
+    <t>BTN_FLC</t>
+  </si>
+  <si>
+    <t>BTN_NOSE_DN</t>
+  </si>
+  <si>
+    <t>BTN_PAN_UP</t>
+  </si>
+  <si>
+    <t>BTN_PAN_LEFT</t>
+  </si>
+  <si>
+    <t>BTN_PAN_RIGHT</t>
+  </si>
+  <si>
+    <t>BTN_PAN_DN</t>
+  </si>
+  <si>
+    <t>BTN_PAN_SYNC</t>
+  </si>
+  <si>
+    <t>BTN_DIRECT</t>
+  </si>
+  <si>
+    <t>BTN_MENU</t>
+  </si>
+  <si>
+    <t>BTN_FPL</t>
+  </si>
+  <si>
+    <t>BTN_PROC</t>
+  </si>
+  <si>
+    <t>BTN_CLR</t>
+  </si>
+  <si>
+    <t>BTN_ENT</t>
+  </si>
+  <si>
+    <t>Common Bus Encoders</t>
+  </si>
+  <si>
+    <t>Encoder name</t>
+  </si>
+  <si>
+    <t>Encoder code</t>
+  </si>
+  <si>
+    <t>RSG Command Inc</t>
+  </si>
+  <si>
+    <t>RSG Command Dec</t>
+  </si>
+  <si>
+    <t>RSG Command Btn</t>
+  </si>
+  <si>
+    <t>Enc_VOL_LEFT</t>
+  </si>
+  <si>
+    <t>Enc_NAV1</t>
+  </si>
+  <si>
+    <t>Enc_NAV2</t>
+  </si>
+  <si>
+    <t>Enc_HDG</t>
+  </si>
+  <si>
+    <t>Enc_ALT1</t>
+  </si>
+  <si>
+    <t>Enc_ALT2</t>
+  </si>
+  <si>
+    <t>Enc_VOL_RIGHT</t>
+  </si>
+  <si>
+    <t>Enc_COM1</t>
+  </si>
+  <si>
+    <t>Enc_COM2</t>
+  </si>
+  <si>
+    <t>Enc_CRS1</t>
+  </si>
+  <si>
+    <t>Enc_CRS2</t>
+  </si>
+  <si>
+    <t>Enc_FMS1</t>
+  </si>
+  <si>
+    <t>Enc_FMS2</t>
+  </si>
+  <si>
+    <t>BTN_NAV_VOL</t>
+  </si>
+  <si>
+    <t>BTN_FMS</t>
+  </si>
+  <si>
+    <t>BTN_NAV_FF</t>
+  </si>
+  <si>
+    <t>BTN_ALT_SYNC</t>
+  </si>
+  <si>
+    <t>BTN_HDG_SYNC</t>
+  </si>
+  <si>
+    <t>BTN_NAV_TOG</t>
+  </si>
+  <si>
+    <t>BTN_COM_VOL</t>
+  </si>
+  <si>
+    <t>BTN_COM_FF</t>
+  </si>
+  <si>
+    <t>BTN_COM_TOG</t>
+  </si>
+  <si>
+    <t>BTN_CRS_SYNC</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>ENC_NAV_OUTER_UP</t>
+  </si>
+  <si>
+    <t>ENC_NAV_OUTER_DN</t>
+  </si>
+  <si>
+    <t>ENC_NAV_INNER_UP</t>
+  </si>
+  <si>
+    <t>ENC_NAV_INNER_DN</t>
+  </si>
+  <si>
+    <t>ENC_ALT_OUTER_UP</t>
+  </si>
+  <si>
+    <t>ENC_ALT_OUTER_DN</t>
+  </si>
+  <si>
+    <t>ENC_ALT_INNER_UP</t>
+  </si>
+  <si>
+    <t>ENC_ALT_INNER_DN</t>
+  </si>
+  <si>
+    <t>ENC_HDG_UP</t>
+  </si>
+  <si>
+    <t>ENC_HDG_DN</t>
+  </si>
+  <si>
+    <t>ENC_NAV_VOL_UP</t>
+  </si>
+  <si>
+    <t>ENC_NAV_VOL_DN</t>
+  </si>
+  <si>
+    <t>ENC_FMS_INNER_UP</t>
+  </si>
+  <si>
+    <t>ENC_FMS_INNER_DN</t>
+  </si>
+  <si>
+    <t>ENC_FMS_OUTER_UP</t>
+  </si>
+  <si>
+    <t>ENC_FMS_OUTER_DN</t>
+  </si>
+  <si>
+    <t>ENC_RANGE_UP</t>
+  </si>
+  <si>
+    <t>ENC_RANGE_DN</t>
+  </si>
+  <si>
+    <t>Enc_Range</t>
+  </si>
+  <si>
+    <t>ENC_BARO_UP</t>
+  </si>
+  <si>
+    <t>ENC_BARO_DN</t>
+  </si>
+  <si>
+    <t>ENC_CRS_UP</t>
+  </si>
+  <si>
+    <t>ENC_CRS_DN</t>
+  </si>
+  <si>
+    <t>ENC_COM_OUTER_UP</t>
+  </si>
+  <si>
+    <t>ENC_COM_OUTER_DN</t>
+  </si>
+  <si>
+    <t>ENC_COM_INNER_UP</t>
+  </si>
+  <si>
+    <t>ENC_COM_INNER_DN</t>
+  </si>
+  <si>
+    <t>ENC_COM_VOL_UP</t>
+  </si>
+  <si>
+    <t>ENC_COM_VOL_DN</t>
   </si>
 </sst>
 </file>
@@ -487,7 +772,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -521,33 +806,356 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -892,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M89"/>
+  <dimension ref="A2:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84:T100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,28 +1512,31 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.28515625" customWidth="1"/>
     <col min="4" max="4" width="69.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -936,7 +1547,7 @@
       <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -947,7 +1558,7 @@
       <c r="C5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -956,7 +1567,7 @@
       <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -965,7 +1576,7 @@
       <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -976,7 +1587,7 @@
       <c r="C8" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -985,7 +1596,7 @@
       <c r="C9" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>97</v>
       </c>
     </row>
@@ -996,7 +1607,7 @@
       <c r="C10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1005,7 +1616,7 @@
       <c r="C11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1014,8 +1625,8 @@
       <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="M12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1024,8 +1635,8 @@
       <c r="C13" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="M13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1034,8 +1645,8 @@
       <c r="C14" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="M14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1044,8 +1655,8 @@
       <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="M15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1054,8 +1665,8 @@
       <c r="C16" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="M16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1064,8 +1675,8 @@
       <c r="C17" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="M17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1074,8 +1685,8 @@
       <c r="C18" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="M18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1084,8 +1695,8 @@
       <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="M19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1094,8 +1705,8 @@
       <c r="C20" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="M20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1104,8 +1715,8 @@
       <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="M21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1114,10 +1725,10 @@
       <c r="C22" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="M22" s="6"/>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1126,10 +1737,10 @@
       <c r="C23" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="M23" s="6"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1138,8 +1749,8 @@
       <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="M24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1148,7 +1759,7 @@
       <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="6" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1159,7 +1770,7 @@
       <c r="C26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1168,7 +1779,7 @@
       <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1177,7 +1788,7 @@
       <c r="C28" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1186,7 +1797,7 @@
       <c r="C29" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1195,7 +1806,7 @@
       <c r="C30" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1204,7 +1815,7 @@
       <c r="C31" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1213,37 +1824,42 @@
       <c r="C32" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1259,8 +1875,11 @@
       <c r="E36" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1276,8 +1895,11 @@
       <c r="E37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1293,8 +1915,11 @@
       <c r="E38" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1310,8 +1935,11 @@
       <c r="E39" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1327,8 +1955,11 @@
       <c r="E40" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1344,8 +1975,11 @@
       <c r="E41" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1362,7 +1996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8</v>
       </c>
@@ -1378,8 +2012,11 @@
       <c r="E43" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>21</v>
       </c>
@@ -1395,8 +2032,11 @@
       <c r="E44" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>22</v>
       </c>
@@ -1413,7 +2053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>23</v>
       </c>
@@ -1429,8 +2069,11 @@
       <c r="E46" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>24</v>
       </c>
@@ -1446,8 +2089,11 @@
       <c r="E47" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>25</v>
       </c>
@@ -1463,8 +2109,11 @@
       <c r="E48" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>26</v>
       </c>
@@ -1480,8 +2129,11 @@
       <c r="E49" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>27</v>
       </c>
@@ -1497,8 +2149,11 @@
       <c r="E50" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>28</v>
       </c>
@@ -1514,33 +2169,41 @@
       <c r="E51" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="F51" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -1556,8 +2219,11 @@
       <c r="E55" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1573,8 +2239,11 @@
       <c r="E56" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1590,8 +2259,11 @@
       <c r="E57" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -1607,8 +2279,11 @@
       <c r="E58" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5</v>
       </c>
@@ -1624,8 +2299,11 @@
       <c r="E59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6</v>
       </c>
@@ -1641,8 +2319,11 @@
       <c r="E60" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7</v>
       </c>
@@ -1659,7 +2340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8</v>
       </c>
@@ -1676,7 +2357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>21</v>
       </c>
@@ -1693,7 +2374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>22</v>
       </c>
@@ -1710,7 +2391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>23</v>
       </c>
@@ -1726,8 +2407,11 @@
       <c r="E65" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>24</v>
       </c>
@@ -1743,8 +2427,11 @@
       <c r="E66" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>25</v>
       </c>
@@ -1760,8 +2447,11 @@
       <c r="E67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>26</v>
       </c>
@@ -1777,8 +2467,11 @@
       <c r="E68" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>27</v>
       </c>
@@ -1794,8 +2487,11 @@
       <c r="E69" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>28</v>
       </c>
@@ -1811,33 +2507,41 @@
       <c r="E70" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="F70" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1853,8 +2557,11 @@
       <c r="E74" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2</v>
       </c>
@@ -1870,8 +2577,11 @@
       <c r="E75" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -1888,7 +2598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4</v>
       </c>
@@ -1904,8 +2614,11 @@
       <c r="E77" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5</v>
       </c>
@@ -1921,8 +2634,11 @@
       <c r="E78" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>6</v>
       </c>
@@ -1938,8 +2654,11 @@
       <c r="E79" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>7</v>
       </c>
@@ -1955,8 +2674,11 @@
       <c r="E80" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>8</v>
       </c>
@@ -1972,8 +2694,11 @@
       <c r="E81" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>21</v>
       </c>
@@ -1990,7 +2715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>22</v>
       </c>
@@ -2007,7 +2732,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>23</v>
       </c>
@@ -2024,7 +2749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>24</v>
       </c>
@@ -2041,7 +2766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>25</v>
       </c>
@@ -2057,8 +2782,11 @@
       <c r="E86" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>26</v>
       </c>
@@ -2074,8 +2802,11 @@
       <c r="E87" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>27</v>
       </c>
@@ -2091,8 +2822,11 @@
       <c r="E88" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
       </c>
@@ -2108,50 +2842,363 @@
       <c r="E89" t="s">
         <v>49</v>
       </c>
+      <c r="F89" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93">
+        <v>100</v>
+      </c>
+      <c r="E93" t="s">
+        <v>212</v>
+      </c>
+      <c r="F93" t="s">
+        <v>213</v>
+      </c>
+      <c r="G93" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>179</v>
+      </c>
+      <c r="D94">
+        <v>200</v>
+      </c>
+      <c r="E94" t="s">
+        <v>202</v>
+      </c>
+      <c r="F94" t="s">
+        <v>203</v>
+      </c>
+      <c r="G94" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95">
+        <v>300</v>
+      </c>
+      <c r="E95" t="s">
+        <v>204</v>
+      </c>
+      <c r="F95" t="s">
+        <v>205</v>
+      </c>
+      <c r="G95" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96">
+        <v>400</v>
+      </c>
+      <c r="E96" t="s">
+        <v>210</v>
+      </c>
+      <c r="F96" t="s">
+        <v>211</v>
+      </c>
+      <c r="G96" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>182</v>
+      </c>
+      <c r="D97">
+        <v>500</v>
+      </c>
+      <c r="E97" t="s">
+        <v>206</v>
+      </c>
+      <c r="F97" t="s">
+        <v>207</v>
+      </c>
+      <c r="G97" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>183</v>
+      </c>
+      <c r="D98">
+        <v>600</v>
+      </c>
+      <c r="E98" t="s">
+        <v>208</v>
+      </c>
+      <c r="F98" t="s">
+        <v>209</v>
+      </c>
+      <c r="G98" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>184</v>
+      </c>
+      <c r="D99">
+        <v>700</v>
+      </c>
+      <c r="E99" t="s">
+        <v>229</v>
+      </c>
+      <c r="F99" t="s">
+        <v>230</v>
+      </c>
+      <c r="G99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>185</v>
+      </c>
+      <c r="D100">
+        <v>800</v>
+      </c>
+      <c r="E100" t="s">
+        <v>225</v>
+      </c>
+      <c r="F100" t="s">
+        <v>226</v>
+      </c>
+      <c r="G100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>186</v>
+      </c>
+      <c r="D101">
+        <v>900</v>
+      </c>
+      <c r="E101" t="s">
+        <v>227</v>
+      </c>
+      <c r="F101" t="s">
+        <v>228</v>
+      </c>
+      <c r="G101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>187</v>
+      </c>
+      <c r="D102">
+        <v>1000</v>
+      </c>
+      <c r="E102" t="s">
+        <v>221</v>
+      </c>
+      <c r="F102" t="s">
+        <v>222</v>
+      </c>
+      <c r="G102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>188</v>
+      </c>
+      <c r="D103">
+        <v>1100</v>
+      </c>
+      <c r="E103" t="s">
+        <v>223</v>
+      </c>
+      <c r="F103" t="s">
+        <v>224</v>
+      </c>
+      <c r="G103" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>189</v>
+      </c>
+      <c r="D104">
+        <v>1200</v>
+      </c>
+      <c r="E104" t="s">
+        <v>214</v>
+      </c>
+      <c r="F104" t="s">
+        <v>215</v>
+      </c>
+      <c r="G104" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105">
+        <v>1300</v>
+      </c>
+      <c r="E105" t="s">
+        <v>216</v>
+      </c>
+      <c r="F105" t="s">
+        <v>217</v>
+      </c>
+      <c r="G105" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>220</v>
+      </c>
+      <c r="D106" t="s">
+        <v>201</v>
+      </c>
+      <c r="E106" t="s">
+        <v>218</v>
+      </c>
+      <c r="F106" t="s">
+        <v>219</v>
+      </c>
+      <c r="G106" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A72:D72"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D21"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D25:D32"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A34:F34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D2 D55:D72 D74:D1048576 D4 D7 D9 D22:D23 D25 D34 D36:D53">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Not connected">
+  <conditionalFormatting sqref="D1:D2 D55:D71 D74:D90 D4 D7 D9 D22:D23 D25 D36:D52 D93:D1048576">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Not connected">
       <formula>NOT(ISERROR(SEARCH("Not connected",D1)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="25">
       <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E51">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Not connected">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Not connected">
       <formula>NOT(ISERROR(SEARCH("Not connected",E36)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="23">
       <formula>LEN(TRIM(E36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E70">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Not connected">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="Not connected">
       <formula>NOT(ISERROR(SEARCH("Not connected",E55)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="21">
       <formula>LEN(TRIM(E55))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E89">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Not connected">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Not connected">
       <formula>NOT(ISERROR(SEARCH("Not connected",E74)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="19">
       <formula>LEN(TRIM(E74))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E104:G105 F103:G103 E93:G102">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(E93))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D93:G101 F103:G103 E102:G102 D102:D103 D104:G106">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="Not applicable">
+      <formula>NOT(ISERROR(SEARCH("Not applicable",D93)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E103">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Not connected">
+      <formula>NOT(ISERROR(SEARCH("Not connected",E103)))</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="15">
+      <formula>LEN(TRIM(E103))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E103">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Not applicable">
+      <formula>NOT(ISERROR(SEARCH("Not applicable",E103)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E106:F106">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(E106))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:K98">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(K86))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:K99">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Not applicable">
+      <formula>NOT(ISERROR(SEARCH("Not applicable",K86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>